<commit_message>
removed a miss tagged citation and re ran plots
</commit_message>
<xml_diff>
--- a/SSM_Perception_scratch.xlsx
+++ b/SSM_Perception_scratch.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d3engineering-my.sharepoint.com/personal/oadamides_d3embedded_com/Documents/Documents/PhD/2023-2024/SSM_Survey_Paper/survey_SSM_robotics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="13_ncr:1_{803CF3A9-0E1F-1E4F-9602-AE187D508B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F3E473A9-BF6A-4518-B1CA-BCEB5499AA29}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{803CF3A9-0E1F-1E4F-9602-AE187D508B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{542530CC-41E8-4009-8AF8-0318D304150E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{69BFFA8D-C89D-4F6E-A34D-B0212540F3CD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="1180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="1181">
   <si>
     <t>Publication Year</t>
   </si>
@@ -3575,6 +3575,9 @@
   </si>
   <si>
     <t>USE_IN_TABLE</t>
+  </si>
+  <si>
+    <t>LiDAR_EX; Indoor navigation; Blind and visually impaired; deep reinforcement learning; Guiding Robot; navigation; UWB Beacon; Verbal instruction; RADAR_EX; 3DTOF_EX; EMBEDDEDLIN_EX; NVIDIACOMPUTE_EX; INTELCOMPUTE_EX</t>
   </si>
 </sst>
 </file>
@@ -4481,7 +4484,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>3</c:v>
@@ -4631,7 +4634,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -5385,7 +5388,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -6146,7 +6149,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -6452,7 +6455,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -6605,7 +6608,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -7397,7 +7400,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>3</c:v>
@@ -7547,7 +7550,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -8301,7 +8304,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -9405,7 +9408,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -9711,7 +9714,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -9864,7 +9867,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -10506,7 +10509,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -10958,7 +10961,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -11410,7 +11413,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5</c:v>
@@ -12049,7 +12052,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>3</c:v>
@@ -12199,7 +12202,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -12953,7 +12956,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -13410,7 +13413,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -13716,7 +13719,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -13869,7 +13872,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -15461,7 +15464,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -21886,8 +21889,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825518CA-F60F-4DC4-87D6-FEDC2F6AE5B4}">
   <dimension ref="A1:BA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AY11" sqref="AY11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V32" sqref="V32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22175,11 +22178,11 @@
       </c>
       <c r="Z2">
         <f>SUM(H2:H101)</f>
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="AA2">
         <f>SUM(I2:I101)</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AB2">
         <f>SUM(J2:J101)</f>
@@ -22199,7 +22202,7 @@
       </c>
       <c r="AF2">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="AG2">
         <f t="shared" si="1"/>
@@ -22219,7 +22222,7 @@
       </c>
       <c r="AK2">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AL2">
         <f t="shared" si="1"/>
@@ -22227,11 +22230,11 @@
       </c>
       <c r="AM2">
         <f t="shared" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN2">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO2">
         <f t="shared" si="1"/>
@@ -24787,11 +24790,11 @@
       </c>
       <c r="Z17">
         <f t="shared" si="20"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AA17">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AB17">
         <f t="shared" si="22"/>
@@ -24811,7 +24814,7 @@
       </c>
       <c r="AF17">
         <f t="shared" si="26"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG17">
         <f t="shared" si="27"/>
@@ -24831,7 +24834,7 @@
       </c>
       <c r="AK17">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL17">
         <f t="shared" si="32"/>
@@ -24839,11 +24842,11 @@
       </c>
       <c r="AM17">
         <f t="shared" si="33"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN17">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO17">
         <f t="shared" si="35"/>
@@ -24858,7 +24861,7 @@
       </c>
       <c r="AR17">
         <f t="shared" si="37"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AS17">
         <f t="shared" si="38"/>
@@ -24866,7 +24869,7 @@
       </c>
       <c r="AT17">
         <f t="shared" si="39"/>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:53" x14ac:dyDescent="0.25">
@@ -26871,7 +26874,7 @@
         <v>55</v>
       </c>
       <c r="E38" t="s">
-        <v>57</v>
+        <v>1180</v>
       </c>
       <c r="G38">
         <f t="shared" si="2"/>
@@ -26879,11 +26882,11 @@
       </c>
       <c r="H38">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <f t="shared" si="5"/>
@@ -26903,7 +26906,7 @@
       </c>
       <c r="N38">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O38">
         <f t="shared" si="10"/>
@@ -26923,7 +26926,7 @@
       </c>
       <c r="S38">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T38">
         <f t="shared" si="15"/>
@@ -26931,11 +26934,11 @@
       </c>
       <c r="U38">
         <f t="shared" si="16"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V38">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W38">
         <f t="shared" si="18"/>

</xml_diff>

<commit_message>
updated data on two miss tagged sources
</commit_message>
<xml_diff>
--- a/SSM_Perception_scratch.xlsx
+++ b/SSM_Perception_scratch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d3engineering-my.sharepoint.com/personal/oadamides_d3embedded_com/Documents/Documents/PhD/2023-2024/SSM_Survey_Paper/survey_SSM_robotics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="13_ncr:1_{803CF3A9-0E1F-1E4F-9602-AE187D508B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{542530CC-41E8-4009-8AF8-0318D304150E}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{803CF3A9-0E1F-1E4F-9602-AE187D508B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BA398E-D2BF-45D7-9F74-BB627F56F80B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{69BFFA8D-C89D-4F6E-A34D-B0212540F3CD}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="1183">
   <si>
     <t>Publication Year</t>
   </si>
@@ -3578,6 +3578,12 @@
   </si>
   <si>
     <t>LiDAR_EX; Indoor navigation; Blind and visually impaired; deep reinforcement learning; Guiding Robot; navigation; UWB Beacon; Verbal instruction; RADAR_EX; 3DTOF_EX; EMBEDDEDLIN_EX; NVIDIACOMPUTE_EX; INTELCOMPUTE_EX</t>
+  </si>
+  <si>
+    <t>Dynamic SSM; Simulation Only</t>
+  </si>
+  <si>
+    <t>Force and tactile sensing; gesture; posture and facial expressions; sensor-based control; PC; IR; BAREMETAL</t>
   </si>
 </sst>
 </file>
@@ -4325,7 +4331,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
@@ -4478,7 +4484,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
@@ -5686,7 +5692,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5</c:v>
@@ -7241,7 +7247,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
@@ -7394,7 +7400,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
@@ -8945,7 +8951,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5</c:v>
@@ -11404,10 +11410,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>4</c:v>
@@ -11893,7 +11899,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>4</c:v>
@@ -12046,7 +12052,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>2</c:v>
@@ -14171,7 +14177,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>5</c:v>
@@ -14707,7 +14713,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>1</c:v>
@@ -21889,8 +21895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825518CA-F60F-4DC4-87D6-FEDC2F6AE5B4}">
   <dimension ref="A1:BA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V32" sqref="V32"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22174,11 +22180,11 @@
       </c>
       <c r="Y2">
         <f>SUM(G2:G101)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z2">
         <f>SUM(H2:H101)</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="AA2">
         <f>SUM(I2:I101)</f>
@@ -22210,7 +22216,7 @@
       </c>
       <c r="AH2">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="AI2">
         <f t="shared" si="1"/>
@@ -24261,7 +24267,7 @@
       </c>
       <c r="Y14">
         <f t="shared" si="19"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z14">
         <f t="shared" si="20"/>
@@ -24336,7 +24342,7 @@
       </c>
       <c r="AR14">
         <f t="shared" si="37"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AS14">
         <f t="shared" si="38"/>
@@ -24440,7 +24446,7 @@
       </c>
       <c r="Z15">
         <f t="shared" si="20"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AA15">
         <f t="shared" si="21"/>
@@ -24472,7 +24478,7 @@
       </c>
       <c r="AH15">
         <f t="shared" si="28"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="AI15">
         <f t="shared" si="29"/>
@@ -24511,11 +24517,11 @@
       </c>
       <c r="AR15">
         <f t="shared" si="37"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AS15">
         <f t="shared" si="38"/>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AT15">
         <f t="shared" si="39"/>
@@ -29184,7 +29190,7 @@
         <v>72</v>
       </c>
       <c r="E65" t="s">
-        <v>74</v>
+        <v>1181</v>
       </c>
       <c r="G65">
         <f t="shared" si="2"/>
@@ -29192,7 +29198,7 @@
       </c>
       <c r="H65">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65">
         <f t="shared" si="4"/>
@@ -29224,7 +29230,7 @@
       </c>
       <c r="P65">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q65">
         <f t="shared" si="12"/>
@@ -30167,11 +30173,11 @@
         <v>48</v>
       </c>
       <c r="E76" t="s">
-        <v>50</v>
+        <v>1182</v>
       </c>
       <c r="G76">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H76">
         <f t="shared" si="41"/>

</xml_diff>

<commit_message>
updated trends.py to expand out 2023 and 2024 years explicitly
</commit_message>
<xml_diff>
--- a/SSM_Perception_scratch.xlsx
+++ b/SSM_Perception_scratch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d3engineering-my.sharepoint.com/personal/oadamides_d3embedded_com/Documents/Documents/PhD/2023-2024/SSM_Survey_Paper/survey_SSM_robotics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{803CF3A9-0E1F-1E4F-9602-AE187D508B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{82BA398E-D2BF-45D7-9F74-BB627F56F80B}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{803CF3A9-0E1F-1E4F-9602-AE187D508B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8A73899-277F-406A-92B0-F050D65543BA}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{69BFFA8D-C89D-4F6E-A34D-B0212540F3CD}"/>
+    <workbookView xWindow="38280" yWindow="-8235" windowWidth="38640" windowHeight="21240" xr2:uid="{69BFFA8D-C89D-4F6E-A34D-B0212540F3CD}"/>
   </bookViews>
   <sheets>
     <sheet name="DataProcessing" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1889" uniqueCount="1186">
   <si>
     <t>Publication Year</t>
   </si>
@@ -3584,6 +3584,15 @@
   </si>
   <si>
     <t>Force and tactile sensing; gesture; posture and facial expressions; sensor-based control; PC; IR; BAREMETAL</t>
+  </si>
+  <si>
+    <t>LiDAR_EX; 3DTOF_EX; MONOVISION_EX; STEREOVISION_EX; PC_EX; sensor performance metrics</t>
+  </si>
+  <si>
+    <t>THERMAL; 3DTOF; PC; Kinect</t>
+  </si>
+  <si>
+    <t>Stereo vision; STEREOVISION_EX; PC_EX</t>
   </si>
 </sst>
 </file>
@@ -4490,10 +4499,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -4640,7 +4649,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -5090,7 +5099,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -5242,13 +5251,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -5698,13 +5707,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -7406,10 +7415,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -7556,7 +7565,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -8006,7 +8015,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -8158,13 +8167,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -8957,13 +8966,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -10515,7 +10524,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -11269,13 +11278,13 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2</c:v>
@@ -11419,10 +11428,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2</c:v>
@@ -12058,10 +12067,10 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0</c:v>
@@ -12208,7 +12217,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1</c:v>
@@ -12658,7 +12667,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0</c:v>
@@ -12810,13 +12819,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>1</c:v>
@@ -14183,13 +14192,13 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>2</c:v>
@@ -15090,7 +15099,7 @@
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
@@ -15467,7 +15476,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -21895,8 +21904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{825518CA-F60F-4DC4-87D6-FEDC2F6AE5B4}">
   <dimension ref="A1:BA116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E72" sqref="E72"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -22188,7 +22197,7 @@
       </c>
       <c r="AA2">
         <f>SUM(I2:I101)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="AB2">
         <f>SUM(J2:J101)</f>
@@ -22200,11 +22209,11 @@
       </c>
       <c r="AD2">
         <f t="shared" ref="AD2:AO2" si="1">SUM(L2:L101)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AE2">
         <f t="shared" si="1"/>
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AF2">
         <f t="shared" si="1"/>
@@ -22216,7 +22225,7 @@
       </c>
       <c r="AH2">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="AI2">
         <f t="shared" si="1"/>
@@ -23495,7 +23504,7 @@
         <v>197</v>
       </c>
       <c r="E10" t="s">
-        <v>198</v>
+        <v>1185</v>
       </c>
       <c r="F10" t="s">
         <v>199</v>
@@ -23526,7 +23535,7 @@
       </c>
       <c r="M10">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N10">
         <f t="shared" si="9"/>
@@ -23538,7 +23547,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q10">
         <f t="shared" si="12"/>
@@ -24796,11 +24805,11 @@
       </c>
       <c r="Z17">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA17">
         <f t="shared" si="21"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AB17">
         <f t="shared" si="22"/>
@@ -24812,11 +24821,11 @@
       </c>
       <c r="AD17">
         <f t="shared" si="24"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AE17">
         <f t="shared" si="25"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AF17">
         <f t="shared" si="26"/>
@@ -24828,7 +24837,7 @@
       </c>
       <c r="AH17">
         <f t="shared" si="28"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AI17">
         <f t="shared" si="29"/>
@@ -24863,15 +24872,15 @@
       </c>
       <c r="AQ17">
         <f t="shared" si="36"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AR17">
         <f t="shared" si="37"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AS17">
         <f t="shared" si="38"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="AT17">
         <f t="shared" si="39"/>
@@ -24971,7 +24980,7 @@
       </c>
       <c r="Z18">
         <f t="shared" si="20"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AA18">
         <f t="shared" si="21"/>
@@ -24991,7 +25000,7 @@
       </c>
       <c r="AE18">
         <f t="shared" si="25"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AF18">
         <f t="shared" si="26"/>
@@ -25038,11 +25047,11 @@
       </c>
       <c r="AQ18">
         <f t="shared" si="36"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AR18">
         <f t="shared" si="37"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AS18">
         <f t="shared" si="38"/>
@@ -25166,7 +25175,7 @@
       </c>
       <c r="AE19">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AF19">
         <f t="shared" si="26"/>
@@ -25178,7 +25187,7 @@
       </c>
       <c r="AH19">
         <f t="shared" si="28"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AI19">
         <f t="shared" si="29"/>
@@ -25213,7 +25222,7 @@
       </c>
       <c r="AQ19">
         <f t="shared" si="36"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="AR19">
         <f t="shared" si="37"/>
@@ -25221,7 +25230,7 @@
       </c>
       <c r="AS19">
         <f t="shared" si="38"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AT19">
         <f t="shared" si="39"/>
@@ -26622,7 +26631,7 @@
         <v>333</v>
       </c>
       <c r="E35" t="s">
-        <v>368</v>
+        <v>1184</v>
       </c>
       <c r="F35" t="s">
         <v>389</v>
@@ -26633,7 +26642,7 @@
       </c>
       <c r="H35">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <f t="shared" si="4"/>
@@ -26653,7 +26662,7 @@
       </c>
       <c r="M35">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35">
         <f t="shared" si="9"/>
@@ -27475,7 +27484,7 @@
         <v>168</v>
       </c>
       <c r="E45" t="s">
-        <v>169</v>
+        <v>1183</v>
       </c>
       <c r="G45">
         <f t="shared" si="2"/>
@@ -27483,11 +27492,11 @@
       </c>
       <c r="H45">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45">
         <f t="shared" si="4"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J45">
         <f t="shared" si="5"/>
@@ -27499,11 +27508,11 @@
       </c>
       <c r="L45">
         <f t="shared" si="7"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N45">
         <f t="shared" si="9"/>
@@ -27515,7 +27524,7 @@
       </c>
       <c r="P45">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q45">
         <f t="shared" si="12"/>

</xml_diff>